<commit_message>
Adding cleaned wine_data.csv with the strange characters removed. Also adding updates to data_week1 file.
</commit_message>
<xml_diff>
--- a/data_cleaning/characters_to_change.xlsx
+++ b/data_cleaning/characters_to_change.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SE\um\hw\20\Mod20_Group_Challenge\data_cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E168DB-F1F8-44CC-8F83-E09BE2236FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C7DE40-28F7-407A-974C-E074A4F7BF22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="1080" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="810" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
   <si>
     <t>Ã</t>
   </si>
@@ -45,149 +55,242 @@
     <t>à</t>
   </si>
   <si>
+    <t>apostraphe</t>
+  </si>
+  <si>
+    <t>Ã¼</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>ü</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Ã©</t>
+  </si>
+  <si>
+    <t>è</t>
+  </si>
+  <si>
+    <t>Ã¶</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>ö</t>
+  </si>
+  <si>
+    <t>Ã¬</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>ì</t>
+  </si>
+  <si>
+    <t>Ã¨</t>
+  </si>
+  <si>
+    <t>Ã¢</t>
+  </si>
+  <si>
+    <t>â</t>
+  </si>
+  <si>
+    <t>Ã±</t>
+  </si>
+  <si>
+    <t>ñ</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>í</t>
+  </si>
+  <si>
+    <t>Ã¥</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>å</t>
+  </si>
+  <si>
+    <t>ò</t>
+  </si>
+  <si>
+    <t>Ã³</t>
+  </si>
+  <si>
+    <t>Ã‰</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>É</t>
+  </si>
+  <si>
+    <t>ç</t>
+  </si>
+  <si>
+    <t>ã</t>
+  </si>
+  <si>
+    <t>Ã§</t>
+  </si>
+  <si>
+    <t>Ãµ</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>ô</t>
+  </si>
+  <si>
+    <t>Ã´</t>
+  </si>
+  <si>
+    <t>Ã¡</t>
+  </si>
+  <si>
+    <t>á</t>
+  </si>
+  <si>
+    <t>ó</t>
+  </si>
+  <si>
+    <t>Ã¤</t>
+  </si>
+  <si>
+    <t>ae</t>
+  </si>
+  <si>
+    <t>ä</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ã </t>
+  </si>
+  <si>
+    <t>oe</t>
+  </si>
+  <si>
+    <t>Ãº</t>
+  </si>
+  <si>
+    <t>ú</t>
+  </si>
+  <si>
+    <t>Ã-</t>
+  </si>
+  <si>
+    <t>Ã¿</t>
+  </si>
+  <si>
+    <t>ÿ</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Ã£</t>
+  </si>
+  <si>
+    <t>ï</t>
+  </si>
+  <si>
+    <t>Ã¯</t>
+  </si>
+  <si>
+    <t>Ã¹</t>
+  </si>
+  <si>
+    <t>Î</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Ã²</t>
+  </si>
+  <si>
+    <t>ÃŽ</t>
+  </si>
+  <si>
+    <t>Ã®</t>
+  </si>
+  <si>
+    <t>î</t>
+  </si>
+  <si>
+    <t>Ã€</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Á</t>
+  </si>
+  <si>
+    <t>RÃ­as Baixas</t>
+  </si>
+  <si>
+    <t>Rias Baixas</t>
+  </si>
+  <si>
+    <t>Ãœ</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Ã–</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Ãª</t>
+  </si>
+  <si>
+    <t>PrÃ­ncipe</t>
+  </si>
+  <si>
+    <t>Principe</t>
+  </si>
+  <si>
+    <t>Ã»</t>
+  </si>
+  <si>
     <t>â€™</t>
   </si>
   <si>
-    <t>apostraphe</t>
-  </si>
-  <si>
-    <t>Ã¼</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>ü</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Ã©</t>
-  </si>
-  <si>
-    <t>è</t>
-  </si>
-  <si>
-    <t>Ã¶</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>ö</t>
-  </si>
-  <si>
-    <t>Ã¬</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>ì</t>
-  </si>
-  <si>
-    <t>Ã¨</t>
-  </si>
-  <si>
-    <t>Ã¢</t>
-  </si>
-  <si>
-    <t>â</t>
-  </si>
-  <si>
-    <t>Ã±</t>
-  </si>
-  <si>
-    <t>ñ</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>í</t>
-  </si>
-  <si>
-    <t>Ã¥</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>å</t>
-  </si>
-  <si>
-    <t>ò</t>
-  </si>
-  <si>
-    <t>Ã³</t>
-  </si>
-  <si>
-    <t>Ã‰</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>É</t>
-  </si>
-  <si>
-    <t>ç</t>
-  </si>
-  <si>
-    <t>ã</t>
-  </si>
-  <si>
-    <t>Ã§</t>
-  </si>
-  <si>
-    <t>Ãµ</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>ô</t>
-  </si>
-  <si>
-    <t>Ã´</t>
-  </si>
-  <si>
-    <t>Ã¡</t>
-  </si>
-  <si>
-    <t>á</t>
-  </si>
-  <si>
-    <t>ó</t>
-  </si>
-  <si>
-    <t>Ã¤</t>
-  </si>
-  <si>
-    <t>ae</t>
-  </si>
-  <si>
-    <t>ä</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ã </t>
-  </si>
-  <si>
-    <t>oe</t>
-  </si>
-  <si>
-    <t>Ãº</t>
-  </si>
-  <si>
-    <t>ú</t>
+    <t>Aldas</t>
+  </si>
+  <si>
+    <t>Aguila</t>
+  </si>
+  <si>
+    <t>Ambar</t>
+  </si>
+  <si>
+    <t>lâ€”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +329,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF5F6368"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5F6368"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -248,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -266,6 +388,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +696,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -581,89 +706,89 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
+      <c r="A3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -671,121 +796,272 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="4" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>51</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>